<commit_message>
Added residual blocks to improve accuracy.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="2i" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
-    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
+    <sheet name="convol_only" sheetId="1" r:id="rId1"/>
+    <sheet name="residual_conn" sheetId="4" r:id="rId2"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId3"/>
+    <sheet name="Лист3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>init_filters</t>
   </si>
@@ -40,6 +41,24 @@
   </si>
   <si>
     <t>Hyperband</t>
+  </si>
+  <si>
+    <t>Bayes</t>
+  </si>
+  <si>
+    <t>val_accuracy</t>
+  </si>
+  <si>
+    <t>Training did not finish due to usage limits</t>
+  </si>
+  <si>
+    <t>Manual. 2nd round</t>
+  </si>
+  <si>
+    <t>num_resid</t>
+  </si>
+  <si>
+    <t>Second attempt</t>
   </si>
 </sst>
 </file>
@@ -50,7 +69,7 @@
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,6 +84,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -88,7 +114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -112,6 +138,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -417,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,7 +460,7 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -672,13 +701,212 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="52.5703125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>32</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.96153146028518599</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>32</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.963708937168121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>64</v>
+      </c>
+      <c r="B6" s="1">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>5</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.96588641405105502</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>6</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.96550000000000002</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1">
+        <v>6</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.95772093534469604</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>64</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>7</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.963708937168121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>64</v>
+      </c>
+      <c r="B11" s="1">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1">
+        <v>6</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0.96606785058975198</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>64</v>
+      </c>
+      <c r="B12" s="1">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1">
+        <v>6</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0.96516060829162598</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>16</v>
+      </c>
+      <c r="B13" s="1">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1">
+        <v>6</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.96570497751235895</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>64</v>
+      </c>
+      <c r="B14" s="1">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1">
+        <v>6</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0.96407186985015803</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -692,4 +920,16 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
An attempt to add batch normalization but accuracy got worse.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>init_filters</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>Second attempt</t>
+  </si>
+  <si>
+    <t>Batch normalization</t>
   </si>
 </sst>
 </file>
@@ -701,10 +704,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,6 +906,48 @@
       <c r="D14" s="4">
         <v>0.96407186985015803</v>
       </c>
+    </row>
+    <row r="16" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1">
+        <v>6</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0.96243876218795699</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>64</v>
+      </c>
+      <c r="B18" s="1">
+        <v>4</v>
+      </c>
+      <c r="C18" s="1">
+        <v>6</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0.96316456794738703</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="9"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>